<commit_message>
Added new exercises and labs in Programming Fundamentals
</commit_message>
<xml_diff>
--- a/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
+++ b/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
   <si>
     <t>Programming Fundamentals - Extended</t>
   </si>
@@ -286,12 +286,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -405,59 +413,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -469,80 +477,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -965,7 +979,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,15 +993,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1096,7 +1110,7 @@
       <c r="B6" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="46">
         <f>C5+1</f>
         <v>42883</v>
       </c>
@@ -1107,7 +1121,7 @@
       <c r="E6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="48" t="str">
+      <c r="F6" s="47" t="str">
         <f t="shared" si="1"/>
         <v>Preslav</v>
       </c>
@@ -1116,24 +1130,24 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="37">
         <f>C6+2</f>
         <v>42885</v>
       </c>
-      <c r="D7" s="9" t="str">
+      <c r="D7" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="13" t="str">
+      <c r="E7" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
@@ -1163,7 +1177,7 @@
         <f t="shared" si="1"/>
         <v>Preslav</v>
       </c>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="45" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1189,7 +1203,9 @@
         <f t="shared" si="1"/>
         <v>Preslav</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" s="50" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="10" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">

</xml_diff>

<commit_message>
Added Data Types & Variables - Exercises
</commit_message>
<xml_diff>
--- a/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
+++ b/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
   <si>
     <t>Programming Fundamentals - Extended</t>
   </si>
@@ -286,12 +286,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -413,59 +421,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -477,83 +485,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -979,7 +990,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,15 +1004,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1203,7 +1214,7 @@
         <f t="shared" si="1"/>
         <v>Preslav</v>
       </c>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="49" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1229,7 +1240,9 @@
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="51" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="11" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">

</xml_diff>

<commit_message>
Programming Fundamentals - Extended - A Lab
</commit_message>
<xml_diff>
--- a/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
+++ b/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="87">
   <si>
     <t>Programming Fundamentals - Extended</t>
   </si>
@@ -286,12 +286,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -423,57 +431,54 @@
   </cellStyleXfs>
   <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -482,89 +487,92 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -990,7 +998,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,928 +1046,930 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="31">
         <v>42878</v>
       </c>
-      <c r="D3" s="37" t="str">
+      <c r="D3" s="32" t="str">
         <f t="shared" ref="D3:D22" si="0">TEXT(C3,"dddd")</f>
         <v>Tuesday</v>
       </c>
-      <c r="E3" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="38" t="str">
+      <c r="E3" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="33" t="str">
         <f t="shared" ref="F3:F39" si="1">IF(OR(D3="Saturday", D3="Sunday"), "Preslav", "Team")</f>
         <v>Team</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40">
+    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="31">
         <f>C3</f>
         <v>42878</v>
       </c>
-      <c r="D4" s="41" t="str">
+      <c r="D4" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="E4" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="38" t="str">
+      <c r="E4" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="33" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42">
+    <row r="5" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37">
         <v>1.2</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="31">
         <f>C4+4</f>
         <v>42882</v>
       </c>
-      <c r="D5" s="37" t="str">
+      <c r="D5" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="E5" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G5" s="33" t="s">
+      <c r="E5" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G5" s="28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+    <row r="6" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="41">
         <f>C5+1</f>
         <v>42883</v>
       </c>
-      <c r="D6" s="41" t="str">
+      <c r="D6" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="E6" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="47" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G6" s="39" t="s">
+      <c r="E6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="42" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G6" s="34" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+    <row r="7" spans="1:7" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="32">
         <f>C6+2</f>
         <v>42885</v>
       </c>
-      <c r="D7" s="37" t="str">
+      <c r="D7" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="E7" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="38" t="str">
+      <c r="E7" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="33" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="G7" s="39" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <f>C7+4</f>
         <v>42889</v>
       </c>
-      <c r="D8" s="9" t="str">
+      <c r="D8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G8" s="45" t="s">
+      <c r="E8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G8" s="40" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <f t="shared" ref="C9" si="2">C8+1</f>
         <v>42890</v>
       </c>
-      <c r="D9" s="28" t="str">
+      <c r="D9" s="24" t="str">
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G9" s="49" t="s">
+      <c r="E9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G9" s="44" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <f t="shared" ref="C10" si="3">C9+2</f>
         <v>42892</v>
       </c>
-      <c r="D10" s="9" t="str">
+      <c r="D10" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="13" t="str">
+      <c r="E10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="45" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="47">
         <f t="shared" ref="C11" si="4">C10+4</f>
         <v>42896</v>
       </c>
-      <c r="D11" s="32" t="str">
+      <c r="D11" s="36" t="str">
         <f>TEXT(C11,"dddd")</f>
         <v>Saturday</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="22" t="str">
+      <c r="E11" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="49" t="str">
         <f>IF(OR(D11="Saturday", D11="Sunday"), "Preslav", "Team")</f>
         <v>Preslav</v>
       </c>
-      <c r="G11" s="24"/>
-    </row>
-    <row r="12" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="G11" s="51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <f t="shared" ref="C12:C39" si="5">C11+1</f>
         <v>42897</v>
       </c>
-      <c r="D12" s="28" t="str">
+      <c r="D12" s="24" t="str">
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="E12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <f t="shared" ref="C13:C37" si="6">C12+2</f>
         <v>42899</v>
       </c>
-      <c r="D13" s="9" t="str">
+      <c r="D13" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="13" t="str">
+      <c r="E13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="19">
         <f t="shared" ref="C14:C38" si="7">C13+4</f>
         <v>42903</v>
       </c>
-      <c r="D14" s="9" t="str">
+      <c r="D14" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="E14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <f t="shared" si="5"/>
         <v>42904</v>
       </c>
-      <c r="D15" s="28" t="str">
+      <c r="D15" s="24" t="str">
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="E15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <f t="shared" si="6"/>
         <v>42906</v>
       </c>
-      <c r="D16" s="9" t="str">
+      <c r="D16" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="13" t="str">
+      <c r="E16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <f t="shared" si="7"/>
         <v>42910</v>
       </c>
-      <c r="D17" s="9" t="str">
+      <c r="D17" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="E17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <f t="shared" si="5"/>
         <v>42911</v>
       </c>
-      <c r="D18" s="28" t="str">
+      <c r="D18" s="24" t="str">
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="E18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <f t="shared" si="6"/>
         <v>42913</v>
       </c>
-      <c r="D19" s="9" t="str">
+      <c r="D19" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="13" t="str">
+      <c r="E19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="19">
         <f t="shared" si="7"/>
         <v>42917</v>
       </c>
-      <c r="D20" s="9" t="str">
+      <c r="D20" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="E20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <f t="shared" si="5"/>
         <v>42918</v>
       </c>
-      <c r="D21" s="28" t="str">
+      <c r="D21" s="24" t="str">
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="E21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <f t="shared" si="6"/>
         <v>42920</v>
       </c>
-      <c r="D22" s="9" t="str">
+      <c r="D22" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="13" t="str">
+      <c r="E22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="19">
         <f t="shared" si="7"/>
         <v>42924</v>
       </c>
-      <c r="D23" s="29" t="str">
+      <c r="D23" s="25" t="str">
         <f>TEXT(C23,"dddd")</f>
         <v>Saturday</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="E23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <f t="shared" si="5"/>
         <v>42925</v>
       </c>
-      <c r="D24" s="15" t="str">
+      <c r="D24" s="14" t="str">
         <f t="shared" ref="D24:D39" si="8">TEXT(C24,"dddd")</f>
         <v>Sunday</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="E24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <f t="shared" si="6"/>
         <v>42927</v>
       </c>
-      <c r="D25" s="29" t="str">
+      <c r="D25" s="25" t="str">
         <f t="shared" si="8"/>
         <v>Tuesday</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="11" t="str">
+      <c r="E25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G25" s="12"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="19">
         <f t="shared" si="7"/>
         <v>42931</v>
       </c>
-      <c r="D26" s="10" t="str">
+      <c r="D26" s="9" t="str">
         <f t="shared" si="8"/>
         <v>Saturday</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G26" s="12"/>
+      <c r="E26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="9">
         <f t="shared" si="5"/>
         <v>42932</v>
       </c>
-      <c r="D27" s="10" t="str">
+      <c r="D27" s="9" t="str">
         <f t="shared" si="8"/>
         <v>Sunday</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G27" s="12"/>
-    </row>
-    <row r="28" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="E27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <f t="shared" si="6"/>
         <v>42934</v>
       </c>
-      <c r="D28" s="29" t="str">
+      <c r="D28" s="25" t="str">
         <f t="shared" si="8"/>
         <v>Tuesday</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="11" t="str">
+      <c r="E28" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G28" s="12"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="19">
         <f t="shared" si="7"/>
         <v>42938</v>
       </c>
-      <c r="D29" s="10" t="str">
+      <c r="D29" s="9" t="str">
         <f t="shared" si="8"/>
         <v>Saturday</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G29" s="12"/>
-    </row>
-    <row r="30" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="E29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <f t="shared" si="5"/>
         <v>42939</v>
       </c>
-      <c r="D30" s="29" t="str">
+      <c r="D30" s="25" t="str">
         <f t="shared" si="8"/>
         <v>Sunday</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G30" s="12"/>
-    </row>
-    <row r="31" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="E30" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="8">
         <f t="shared" si="6"/>
         <v>42941</v>
       </c>
-      <c r="D31" s="10" t="str">
+      <c r="D31" s="9" t="str">
         <f t="shared" si="8"/>
         <v>Tuesday</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="11" t="str">
+      <c r="E31" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G31" s="12"/>
-    </row>
-    <row r="32" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="19">
         <f t="shared" si="7"/>
         <v>42945</v>
       </c>
-      <c r="D32" s="29" t="str">
+      <c r="D32" s="25" t="str">
         <f t="shared" si="8"/>
         <v>Saturday</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G32" s="12"/>
-    </row>
-    <row r="33" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="E32" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="9">
         <f t="shared" si="5"/>
         <v>42946</v>
       </c>
-      <c r="D33" s="10" t="str">
+      <c r="D33" s="9" t="str">
         <f t="shared" si="8"/>
         <v>Sunday</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G33" s="12"/>
-    </row>
-    <row r="34" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="E33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8">
         <f t="shared" si="6"/>
         <v>42948</v>
       </c>
-      <c r="D34" s="10" t="str">
+      <c r="D34" s="9" t="str">
         <f t="shared" si="8"/>
         <v>Tuesday</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="11" t="str">
+      <c r="E34" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G34" s="12"/>
-    </row>
-    <row r="35" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="19">
         <f t="shared" si="7"/>
         <v>42952</v>
       </c>
-      <c r="D35" s="29" t="str">
+      <c r="D35" s="25" t="str">
         <f t="shared" si="8"/>
         <v>Saturday</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G35" s="12"/>
+      <c r="E35" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="9">
         <f t="shared" si="5"/>
         <v>42953</v>
       </c>
-      <c r="D36" s="10" t="str">
+      <c r="D36" s="9" t="str">
         <f t="shared" si="8"/>
         <v>Sunday</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G36" s="12"/>
-    </row>
-    <row r="37" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="E36" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8">
         <f t="shared" si="6"/>
         <v>42955</v>
       </c>
-      <c r="D37" s="10" t="str">
+      <c r="D37" s="9" t="str">
         <f t="shared" si="8"/>
         <v>Tuesday</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="11" t="str">
+      <c r="E37" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G37" s="12"/>
-    </row>
-    <row r="38" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="20">
+      <c r="C38" s="19">
         <f t="shared" si="7"/>
         <v>42959</v>
       </c>
-      <c r="D38" s="10" t="str">
+      <c r="D38" s="9" t="str">
         <f t="shared" si="8"/>
         <v>Saturday</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G38" s="12"/>
-    </row>
-    <row r="39" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="E38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="9">
         <f t="shared" si="5"/>
         <v>42960</v>
       </c>
-      <c r="D39" s="10" t="str">
+      <c r="D39" s="9" t="str">
         <f t="shared" si="8"/>
         <v>Sunday</v>
       </c>
-      <c r="E39" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G39" s="12"/>
-    </row>
-    <row r="40" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="s">
+      <c r="E39" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="21">
+      <c r="C40" s="20">
         <v>42967</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G40" s="30"/>
+      <c r="G40" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added two folders with probglems from Arrays
</commit_message>
<xml_diff>
--- a/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
+++ b/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="87">
   <si>
     <t>Programming Fundamentals - Extended</t>
   </si>
@@ -286,12 +286,28 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -429,56 +445,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -487,80 +503,80 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -572,7 +588,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -997,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,15 +1034,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1274,7 +1296,7 @@
         <f>IF(OR(D11="Saturday", D11="Sunday"), "Preslav", "Team")</f>
         <v>Preslav</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G11" s="50" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1300,7 +1322,9 @@
         <f t="shared" si="1"/>
         <v>Preslav</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="51" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
@@ -1324,7 +1348,9 @@
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="53" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="14" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">

</xml_diff>

<commit_message>
"Added Arrays - More Exercises"
</commit_message>
<xml_diff>
--- a/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
+++ b/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
   <si>
     <t>Programming Fundamentals - Extended</t>
   </si>
@@ -286,12 +286,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -445,56 +453,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -503,80 +511,80 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -588,13 +596,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1020,7 +1034,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,15 +1048,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1327,28 +1341,28 @@
       </c>
     </row>
     <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="32">
         <f t="shared" ref="C13:C37" si="6">C12+2</f>
         <v>42899</v>
       </c>
-      <c r="D13" s="8" t="str">
+      <c r="D13" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="12" t="str">
+      <c r="E13" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="33" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G13" s="53" t="s">
+      <c r="G13" s="52" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1374,7 +1388,9 @@
         <f t="shared" si="1"/>
         <v>Preslav</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="G14" s="55" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="15" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">

</xml_diff>

<commit_message>
Added some files from labs and exercises
</commit_message>
<xml_diff>
--- a/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
+++ b/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
   <si>
     <t>Programming Fundamentals - Extended</t>
   </si>
@@ -286,12 +286,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -453,56 +461,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -511,105 +519,111 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1034,7 +1048,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,15 +1062,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1388,33 +1402,35 @@
         <f t="shared" si="1"/>
         <v>Preslav</v>
       </c>
-      <c r="G14" s="55" t="s">
+      <c r="G14" s="54" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="41">
         <f t="shared" si="5"/>
         <v>42904</v>
       </c>
-      <c r="D15" s="24" t="str">
+      <c r="D15" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G15" s="11"/>
+      <c r="E15" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G15" s="57" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
@@ -1438,7 +1454,9 @@
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G16" s="11"/>
+      <c r="G16" s="57" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="17" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">

</xml_diff>

<commit_message>
Added Dictionaries - Lab and Exercises
</commit_message>
<xml_diff>
--- a/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
+++ b/Tech Module/Programming Fundamentals - Extended/00. Programming-Fundamentals-Extended-Course-Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
   <si>
     <t>Programming Fundamentals - Extended</t>
   </si>
@@ -286,12 +286,28 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -461,56 +477,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -519,80 +535,80 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -604,26 +620,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1047,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,15 +1084,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1410,7 +1432,7 @@
       <c r="A15" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="55" t="s">
         <v>65</v>
       </c>
       <c r="C15" s="41">
@@ -1428,7 +1450,7 @@
         <f t="shared" si="1"/>
         <v>Preslav</v>
       </c>
-      <c r="G15" s="57" t="s">
+      <c r="G15" s="56" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1454,7 +1476,7 @@
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G16" s="57" t="s">
+      <c r="G16" s="56" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1480,55 +1502,61 @@
         <f t="shared" si="1"/>
         <v>Preslav</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="57" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="18" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="41">
         <f t="shared" si="5"/>
         <v>42911</v>
       </c>
-      <c r="D18" s="24" t="str">
+      <c r="D18" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v>Preslav</v>
-      </c>
-      <c r="G18" s="11"/>
+      <c r="E18" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v>Preslav</v>
+      </c>
+      <c r="G18" s="57" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="19" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="32">
         <f t="shared" si="6"/>
         <v>42913</v>
       </c>
-      <c r="D19" s="8" t="str">
+      <c r="D19" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="12" t="str">
+      <c r="E19" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="33" t="str">
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G19" s="11"/>
+      <c r="G19" s="57" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="20" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
@@ -1576,7 +1604,9 @@
         <f t="shared" si="1"/>
         <v>Preslav</v>
       </c>
-      <c r="G21" s="11"/>
+      <c r="G21" s="59" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="22" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
@@ -1600,7 +1630,9 @@
         <f t="shared" si="1"/>
         <v>Team</v>
       </c>
-      <c r="G22" s="11"/>
+      <c r="G22" s="59" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="23" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">

</xml_diff>